<commit_message>
feat: change to correct rouge
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -22,10 +22,10 @@
     <t>system</t>
   </si>
   <si>
-    <t>mean_rouge1_f</t>
-  </si>
-  <si>
-    <t>std_rouge1_f</t>
+    <t>mean_rougel_f</t>
+  </si>
+  <si>
+    <t>std_rougel_f</t>
   </si>
   <si>
     <t>mean_meteor_score</t>
@@ -85,94 +85,94 @@
     <t>codetrans_mt_tf_small_none_bleu_ft</t>
   </si>
   <si>
-    <t>0,43817861762920973</t>
-  </si>
-  <si>
-    <t>0,4411206360931978</t>
-  </si>
-  <si>
-    <t>0,3993272898870669</t>
-  </si>
-  <si>
-    <t>0,47878170031309575</t>
-  </si>
-  <si>
-    <t>0,44893064127955473</t>
-  </si>
-  <si>
-    <t>0,4843121444693881</t>
-  </si>
-  <si>
-    <t>0,40031299606813653</t>
-  </si>
-  <si>
-    <t>0,4395137843063202</t>
-  </si>
-  <si>
-    <t>0,40434914364531555</t>
-  </si>
-  <si>
-    <t>0,4843406057282357</t>
-  </si>
-  <si>
-    <t>0,44634696532648394</t>
-  </si>
-  <si>
-    <t>0,44428104029463217</t>
-  </si>
-  <si>
-    <t>0,4804192766917531</t>
-  </si>
-  <si>
-    <t>0,4355232285201689</t>
-  </si>
-  <si>
-    <t>0,3995149473977877</t>
-  </si>
-  <si>
-    <t>0,26948439889798986</t>
-  </si>
-  <si>
-    <t>0,2615570890809313</t>
-  </si>
-  <si>
-    <t>0,2271498848962539</t>
-  </si>
-  <si>
-    <t>0,294877593792932</t>
-  </si>
-  <si>
-    <t>0,26194307439465386</t>
-  </si>
-  <si>
-    <t>0,2929437791093101</t>
-  </si>
-  <si>
-    <t>0,2263142628651919</t>
-  </si>
-  <si>
-    <t>0,2647463940503955</t>
-  </si>
-  <si>
-    <t>0,23023367769019948</t>
-  </si>
-  <si>
-    <t>0,29358593189687804</t>
-  </si>
-  <si>
-    <t>0,26224886969829125</t>
-  </si>
-  <si>
-    <t>0,26245072996648267</t>
-  </si>
-  <si>
-    <t>0,29523375138112534</t>
-  </si>
-  <si>
-    <t>0,25032797598486645</t>
-  </si>
-  <si>
-    <t>0,22791591476123055</t>
+    <t>0,4135880628838103</t>
+  </si>
+  <si>
+    <t>0,40710156602483993</t>
+  </si>
+  <si>
+    <t>0,36758372684168195</t>
+  </si>
+  <si>
+    <t>0,4546510352479431</t>
+  </si>
+  <si>
+    <t>0,41749451748297195</t>
+  </si>
+  <si>
+    <t>0,4568390471703565</t>
+  </si>
+  <si>
+    <t>0,36843757548969347</t>
+  </si>
+  <si>
+    <t>0,4103334471824482</t>
+  </si>
+  <si>
+    <t>0,36806787051591566</t>
+  </si>
+  <si>
+    <t>0,456952155105607</t>
+  </si>
+  <si>
+    <t>0,4161868475004489</t>
+  </si>
+  <si>
+    <t>0,4099304562893027</t>
+  </si>
+  <si>
+    <t>0,45669792766638645</t>
+  </si>
+  <si>
+    <t>0,40384354391282895</t>
+  </si>
+  <si>
+    <t>0,3677914373223191</t>
+  </si>
+  <si>
+    <t>0,273585971981938</t>
+  </si>
+  <si>
+    <t>0,26825571579833285</t>
+  </si>
+  <si>
+    <t>0,2270243545339394</t>
+  </si>
+  <si>
+    <t>0,30207758652510003</t>
+  </si>
+  <si>
+    <t>0,2672183291578415</t>
+  </si>
+  <si>
+    <t>0,30145102617980485</t>
+  </si>
+  <si>
+    <t>0,22670339508873064</t>
+  </si>
+  <si>
+    <t>0,27039355768925033</t>
+  </si>
+  <si>
+    <t>0,23316500047691527</t>
+  </si>
+  <si>
+    <t>0,3023002624791239</t>
+  </si>
+  <si>
+    <t>0,26752921789007095</t>
+  </si>
+  <si>
+    <t>0,2696637576467272</t>
+  </si>
+  <si>
+    <t>0,3022918320940732</t>
+  </si>
+  <si>
+    <t>0,254215274223736</t>
+  </si>
+  <si>
+    <t>0,22829889400795722</t>
   </si>
   <si>
     <t>0,26368875171137124</t>
@@ -313,34 +313,34 @@
     <t>0,0</t>
   </si>
   <si>
-    <t>0,3556126864086485</t>
-  </si>
-  <si>
-    <t>0,38180686310362044</t>
-  </si>
-  <si>
-    <t>0,36255501181977884</t>
-  </si>
-  <si>
-    <t>0,34255095526501605</t>
-  </si>
-  <si>
-    <t>0,385559105474329</t>
-  </si>
-  <si>
-    <t>0,19947987079106577</t>
-  </si>
-  <si>
-    <t>0,19869700011510646</t>
-  </si>
-  <si>
-    <t>0,18991610380543386</t>
-  </si>
-  <si>
-    <t>0,15946393566107417</t>
-  </si>
-  <si>
-    <t>0,19754077443429385</t>
+    <t>0,3304149838939274</t>
+  </si>
+  <si>
+    <t>0,3482884438287336</t>
+  </si>
+  <si>
+    <t>0,32734240196930287</t>
+  </si>
+  <si>
+    <t>0,3032659666170646</t>
+  </si>
+  <si>
+    <t>0,35020986004032917</t>
+  </si>
+  <si>
+    <t>0,19603554838058318</t>
+  </si>
+  <si>
+    <t>0,1948751835361479</t>
+  </si>
+  <si>
+    <t>0,18506659375230844</t>
+  </si>
+  <si>
+    <t>0,15042429719487305</t>
+  </si>
+  <si>
+    <t>0,1945378727069066</t>
   </si>
   <si>
     <t>0,17832477304277508</t>
@@ -433,94 +433,94 @@
     <t>plbart_camelsnakecase_bleu_ft</t>
   </si>
   <si>
-    <t>0,4739623342107864</t>
-  </si>
-  <si>
-    <t>0,4686270085742361</t>
-  </si>
-  <si>
-    <t>0,46450710985172244</t>
-  </si>
-  <si>
-    <t>0,5169242545484476</t>
-  </si>
-  <si>
-    <t>0,47325761739534666</t>
-  </si>
-  <si>
-    <t>0,5169116135807843</t>
-  </si>
-  <si>
-    <t>0,5156158552902789</t>
-  </si>
-  <si>
-    <t>0,5162339103062558</t>
-  </si>
-  <si>
-    <t>0,4433867667884057</t>
-  </si>
-  <si>
-    <t>0,5041933877918898</t>
-  </si>
-  <si>
-    <t>0,5133752975577188</t>
-  </si>
-  <si>
-    <t>0,44637920837013184</t>
-  </si>
-  <si>
-    <t>0,4454798136256917</t>
-  </si>
-  <si>
-    <t>0,4447284829340655</t>
-  </si>
-  <si>
-    <t>0,5171416167652537</t>
-  </si>
-  <si>
-    <t>0,26887644176311437</t>
-  </si>
-  <si>
-    <t>0,2569797571579843</t>
-  </si>
-  <si>
-    <t>0,25954610524384086</t>
-  </si>
-  <si>
-    <t>0,29339296440419865</t>
-  </si>
-  <si>
-    <t>0,26787627331685304</t>
-  </si>
-  <si>
-    <t>0,2808350516490283</t>
-  </si>
-  <si>
-    <t>0,291872374897986</t>
-  </si>
-  <si>
-    <t>0,29351749760435986</t>
-  </si>
-  <si>
-    <t>0,24174016746785443</t>
-  </si>
-  <si>
-    <t>0,2686526315790876</t>
-  </si>
-  <si>
-    <t>0,278882935624542</t>
-  </si>
-  <si>
-    <t>0,23427831057730114</t>
-  </si>
-  <si>
-    <t>0,23326115844915796</t>
-  </si>
-  <si>
-    <t>0,2346714920011616</t>
-  </si>
-  <si>
-    <t>0,29264267863265536</t>
+    <t>0,4428271805975517</t>
+  </si>
+  <si>
+    <t>0,44077007868241846</t>
+  </si>
+  <si>
+    <t>0,44110618878971314</t>
+  </si>
+  <si>
+    <t>0,4933986961021123</t>
+  </si>
+  <si>
+    <t>0,44266157804112644</t>
+  </si>
+  <si>
+    <t>0,4903718104370656</t>
+  </si>
+  <si>
+    <t>0,4921043414011757</t>
+  </si>
+  <si>
+    <t>0,4897661797317905</t>
+  </si>
+  <si>
+    <t>0,4113543177481951</t>
+  </si>
+  <si>
+    <t>0,47719847420166717</t>
+  </si>
+  <si>
+    <t>0,487165872049073</t>
+  </si>
+  <si>
+    <t>0,4179078949438981</t>
+  </si>
+  <si>
+    <t>0,4170620364778556</t>
+  </si>
+  <si>
+    <t>0,41665098557853886</t>
+  </si>
+  <si>
+    <t>0,49029780455272187</t>
+  </si>
+  <si>
+    <t>0,2766894351597228</t>
+  </si>
+  <si>
+    <t>0,2618179410112169</t>
+  </si>
+  <si>
+    <t>0,2636937177731049</t>
+  </si>
+  <si>
+    <t>0,3012508235213127</t>
+  </si>
+  <si>
+    <t>0,2759802534357222</t>
+  </si>
+  <si>
+    <t>0,2897250214134543</t>
+  </si>
+  <si>
+    <t>0,30010289686379676</t>
+  </si>
+  <si>
+    <t>0,30313109480237155</t>
+  </si>
+  <si>
+    <t>0,24593006779025553</t>
+  </si>
+  <si>
+    <t>0,2764852119782333</t>
+  </si>
+  <si>
+    <t>0,2876688271937383</t>
+  </si>
+  <si>
+    <t>0,2373207047777384</t>
+  </si>
+  <si>
+    <t>0,2358367382523934</t>
+  </si>
+  <si>
+    <t>0,23726232156539284</t>
+  </si>
+  <si>
+    <t>0,3019908964766978</t>
   </si>
   <si>
     <t>0,33751721527482537</t>
@@ -658,34 +658,34 @@
     <t>0,3308416366719033</t>
   </si>
   <si>
-    <t>0,41463470871058705</t>
-  </si>
-  <si>
-    <t>0,40129853157610995</t>
-  </si>
-  <si>
-    <t>0,4000631141947918</t>
-  </si>
-  <si>
-    <t>0,4366212156508629</t>
-  </si>
-  <si>
-    <t>0,43309040301100155</t>
-  </si>
-  <si>
-    <t>0,22139711899090378</t>
-  </si>
-  <si>
-    <t>0,22465694654659307</t>
-  </si>
-  <si>
-    <t>0,2071024368232054</t>
-  </si>
-  <si>
-    <t>0,22732192368627682</t>
-  </si>
-  <si>
-    <t>0,23028043352643052</t>
+    <t>0,3827609327428907</t>
+  </si>
+  <si>
+    <t>0,3776550049208594</t>
+  </si>
+  <si>
+    <t>0,3637469843043001</t>
+  </si>
+  <si>
+    <t>0,40478078157851205</t>
+  </si>
+  <si>
+    <t>0,4030341465129616</t>
+  </si>
+  <si>
+    <t>0,22172419618991876</t>
+  </si>
+  <si>
+    <t>0,22354942556658733</t>
+  </si>
+  <si>
+    <t>0,20617041731096186</t>
+  </si>
+  <si>
+    <t>0,2287514226159065</t>
+  </si>
+  <si>
+    <t>0,23140391793432183</t>
   </si>
   <si>
     <t>0,26938398922076423</t>

</xml_diff>